<commit_message>
Added XIC Measurement/RNAseq measurement
Measurement bias figure suggests that we measure the most ancient proteins more often than the newer proteins. This is the number of proteins measured in each group divided by the number of mRNAs measured in that group.
</commit_message>
<xml_diff>
--- a/Figure2/Proteomics_Core_Analysis/sce_proteins_CoreAnalysis.xlsx
+++ b/Figure2/Proteomics_Core_Analysis/sce_proteins_CoreAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doughty/Documents/GitHub/CHASSY_multiOmics_Analysis/Figure2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doughty/Documents/GitHub/CHASSY_multiOmics_Analysis/Figure2/Proteomics_Core_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0EA3CA0-E297-A841-A724-02AF9CE88A01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F5ABA4-B563-E149-824E-92289A695B2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36560" yWindow="5220" windowWidth="28040" windowHeight="17440" activeTab="5"/>
+    <workbookView xWindow="-36560" yWindow="5220" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sce_SIG_Proteins_Hi_0.75" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="sce_SIG_Proteins_LpH 1" sheetId="6" r:id="rId4"/>
     <sheet name="sce_SIG_Proteins_Osm 0.75" sheetId="4" r:id="rId5"/>
     <sheet name="sce_SIG_Proteins_Osm 1" sheetId="7" r:id="rId6"/>
-    <sheet name="All measured" sheetId="2" r:id="rId7"/>
+    <sheet name="sce_prots_measured" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -4099,7 +4099,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4934,7 +4934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7707,7 +7707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8803,7 +8803,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -10988,7 +10988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11966,7 +11966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16654,10 +16654,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -19511,10 +19511,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G1353"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="F10:G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>